<commit_message>
Amelia, I am pushing my corrected exampledata2Ecruz
</commit_message>
<xml_diff>
--- a/exampledata2Moji.xlsx
+++ b/exampledata2Moji.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{C53D448B-35CF-4E13-BFE7-1AF5A495EE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>